<commit_message>
TEST CASE FOR API TESTED updated.xlsx
</commit_message>
<xml_diff>
--- a/TEST CASE FOR API TESTED updated.xlsx
+++ b/TEST CASE FOR API TESTED updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0a83e89f89a3607f/Desktop/git hub folder/Team-postman-Basic-Github-task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_A8A82C61A3E0154566DBBD16CEBC30A55F4ED415" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF58B938-8E3A-4797-A8F4-052EFB79F1A8}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_A8A82C61A3E0154566DBBD16CEBC30A55F4ED415" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFC35943-E8C1-484F-A3CE-C9AE0C63134A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
   <si>
     <t>TEST CASE FOR DEMOFUSIO</t>
   </si>
@@ -64,15 +64,9 @@
     <t>TC4</t>
   </si>
   <si>
-    <t>confirm that the expected result for  title is "fusio"</t>
-  </si>
-  <si>
     <t>TC5</t>
   </si>
   <si>
-    <t>confirm that body "tittle matches string "fusio"</t>
-  </si>
-  <si>
     <t>TC6</t>
   </si>
   <si>
@@ -85,21 +79,6 @@
     <t>Confirm that entry 5 .rel is Jsonrpc</t>
   </si>
   <si>
-    <t>Confirm that entry 3.rel is root</t>
-  </si>
-  <si>
-    <t>Confirm that entry 6.rel is oauth2</t>
-  </si>
-  <si>
-    <t>Confirm that entry2.rel is documentation</t>
-  </si>
-  <si>
-    <t>Confirm that entry1 is openapi</t>
-  </si>
-  <si>
-    <t>Confirm that entry7 is whoami</t>
-  </si>
-  <si>
     <t>TC7</t>
   </si>
   <si>
@@ -107,13 +86,37 @@
   </si>
   <si>
     <t>Confirm that entry4  is "health"4</t>
+  </si>
+  <si>
+    <t>Confirm that entry1 is "openapi"</t>
+  </si>
+  <si>
+    <t>confirm that entry 7 is "documentation"</t>
+  </si>
+  <si>
+    <t>TC8</t>
+  </si>
+  <si>
+    <t>Confirm that entry 6.rel is "oauth2"</t>
+  </si>
+  <si>
+    <t>Confirm that entry 3.rel is "root"</t>
+  </si>
+  <si>
+    <t>confirm that body "tittle matches string "Fusio"</t>
+  </si>
+  <si>
+    <t>confirm that the expected result for  title is "Fusio"</t>
+  </si>
+  <si>
+    <t>Confirm that entry7 is "whoami"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -139,6 +142,11 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -160,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -171,6 +179,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -186,6 +195,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -392,7 +405,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -456,7 +469,7 @@
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -468,7 +481,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>8</v>
@@ -476,10 +489,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>8</v>
@@ -487,10 +500,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>8</v>
@@ -502,13 +515,13 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>8</v>
@@ -518,8 +531,8 @@
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>21</v>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>8</v>
@@ -530,7 +543,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>8</v>
@@ -549,10 +562,10 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>8</v>
@@ -560,10 +573,10 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>8</v>
@@ -571,24 +584,28 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>24</v>
+      </c>
       <c r="C20" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D20" s="4" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>